<commit_message>
document generated in two foldera
</commit_message>
<xml_diff>
--- a/AppTracker.xlsx
+++ b/AppTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Guest123\GuestRegistrationForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53286525-49B4-41BE-B8AF-CC066F18E32A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C308A-094D-498A-AE5D-713E2BEE67DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -783,7 +783,7 @@
   <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>29</v>

</xml_diff>